<commit_message>
Started filling out BOM
</commit_message>
<xml_diff>
--- a/docs/BOM-golf-gps.xlsx
+++ b/docs/BOM-golf-gps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjkuh\Projects\gitRepos\golf-gps\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepos\golf-gps\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E6D487-791C-4BA7-9F37-3E09A399FDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13846F85-6011-4C3C-B3C7-95D0032E391F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,28 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$H$30</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>Quantity</t>
   </si>
@@ -51,14 +62,293 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Vendor PN</t>
+    <t>Vendor/LCSC PN</t>
+  </si>
+  <si>
+    <t>AE1</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>BT2</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>FB1, FB2</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>C1, C5-8</t>
+  </si>
+  <si>
+    <t>C2, C4</t>
+  </si>
+  <si>
+    <t>C3, C9, C13-16, C19, C20, C23-26</t>
+  </si>
+  <si>
+    <t>C11, C17, C18</t>
+  </si>
+  <si>
+    <t>C21,22</t>
+  </si>
+  <si>
+    <t>C10, C12</t>
+  </si>
+  <si>
+    <t>D2, D3, D5</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>R2, R6</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5, R10-15</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2-5</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>STM32L432KCU6</t>
+  </si>
+  <si>
+    <t>C1337280</t>
+  </si>
+  <si>
+    <t>UFQFPN-32</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 256KB FLSH 32UFQFPN</t>
+  </si>
+  <si>
+    <t>USB4110-GF-A</t>
+  </si>
+  <si>
+    <t>2073-USB4110-GF-A-1-ND</t>
+  </si>
+  <si>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>CONN RCP USB2.0 TYP C 24P SMD RA</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>C3284251</t>
+  </si>
+  <si>
+    <t>RF ANT GNSS PATCH L1 12X12 SMD</t>
+  </si>
+  <si>
+    <t>TE Connectivity Linx</t>
+  </si>
+  <si>
+    <t>ANT-GNSSCP-SM12L1</t>
+  </si>
+  <si>
+    <t>CR2032 Coin Cell Battery Holder</t>
+  </si>
+  <si>
+    <t>PRTR5V0U2X</t>
+  </si>
+  <si>
+    <t>C2827688</t>
+  </si>
+  <si>
+    <t>SOT-143</t>
+  </si>
+  <si>
+    <t>TECH PUBLIC</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5.5VWM SOT143B</t>
+  </si>
+  <si>
+    <t>ETG</t>
+  </si>
+  <si>
+    <t>C424093</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OT</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
+    <t>IC BATT CNTL LI-ION 1CEL SOT23-5</t>
+  </si>
+  <si>
+    <t>Connector for 1.8" TFT LCD from ETG</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 8POS 2.54MM</t>
+  </si>
+  <si>
+    <t>P=2.54mm</t>
+  </si>
+  <si>
+    <t>NEO-M9N</t>
+  </si>
+  <si>
+    <t>C5119087</t>
+  </si>
+  <si>
+    <t>M9 STANDARD PRECISION GNSS MOD</t>
+  </si>
+  <si>
+    <t>U-BLOX</t>
+  </si>
+  <si>
+    <t>SMD-24P</t>
+  </si>
+  <si>
+    <t>X206032768KGB2SC</t>
+  </si>
+  <si>
+    <t>C2236</t>
+  </si>
+  <si>
+    <t>DT-26</t>
+  </si>
+  <si>
+    <t>YXC Crystal Oscillators</t>
+  </si>
+  <si>
+    <t>CRYSTAL 32.7680KHZ 12.5PF TH</t>
+  </si>
+  <si>
+    <t>~1000mAh Lithium Ion Battery</t>
+  </si>
+  <si>
+    <t>BAT54C</t>
+  </si>
+  <si>
+    <t>C2135</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>Jiangsu Changjing Electronics Technology</t>
+  </si>
+  <si>
+    <t>DIODE ARR SCHOTT 30V 200MA SOT23</t>
+  </si>
+  <si>
+    <t>Bel Fuse Inc.</t>
+  </si>
+  <si>
+    <t>0ZCG0050AF2C</t>
+  </si>
+  <si>
+    <t>C3762102</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 30V 500MA 1812</t>
+  </si>
+  <si>
+    <t>EG1218</t>
+  </si>
+  <si>
+    <t>P=2.50mm</t>
+  </si>
+  <si>
+    <t>E-Switch</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 200MA 30V</t>
+  </si>
+  <si>
+    <t>6mm</t>
+  </si>
+  <si>
+    <t>SPDT PUSH BUTTON</t>
+  </si>
+  <si>
+    <t>C15516</t>
+  </si>
+  <si>
+    <t>TPS63031DSKR</t>
+  </si>
+  <si>
+    <t>IC REG BUCK BST 3.3V 900MA 10SON</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>10-WFDFN</t>
+  </si>
+  <si>
+    <t>Total Part Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +393,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -176,8 +474,21 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -490,7 +801,7 @@
     <tableColumn id="1" xr3:uid="{32AFDCD7-F4DF-4ED5-8811-A4897B942137}" name="Quantity" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{FE933B93-DA18-4AED-A480-8EB2CB37E9FA}" name="Reference(s)" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{3756D777-6A0B-46EA-891A-5F8ACDDB5DC3}" name="Part Number" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F268DED4-AA10-4CEF-A3B9-66A35E6F6B34}" name="Vendor PN" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{F268DED4-AA10-4CEF-A3B9-66A35E6F6B34}" name="Vendor/LCSC PN" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{830C4442-5AB3-43AC-A769-0794297CBDA1}" name="Package" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{108683D9-DF72-46B8-9EFA-4A90CB8F9C65}" name="Manufacturer" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{0288C8FE-25DB-42B5-9EE0-77B481F28BD2}" name="Description" dataDxfId="1"/>
@@ -763,23 +1074,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,39 +1118,69 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="7"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
@@ -845,9 +1188,13 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -855,9 +1202,13 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -865,9 +1216,13 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -875,9 +1230,13 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="7"/>
       <c r="E9" s="2"/>
@@ -885,9 +1244,13 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -895,19 +1258,37 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -915,29 +1296,61 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1812</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -945,9 +1358,13 @@
       <c r="G15" s="2"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -955,19 +1372,33 @@
       <c r="G16" s="2"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C17" s="5"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -975,9 +1406,13 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="2"/>
@@ -985,9 +1420,13 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -995,19 +1434,37 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="2"/>
@@ -1015,9 +1472,13 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1025,9 +1486,13 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="12">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1035,9 +1500,13 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="2"/>
@@ -1045,9 +1514,13 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5"/>
       <c r="E26" s="2"/>
@@ -1055,78 +1528,172 @@
       <c r="G26" s="2"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="12">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="12">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="12">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="12">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1135,8 +1702,8 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1145,8 +1712,8 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1154,6 +1721,15 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <f>SUM(A2:A36)</f>
+        <v>64</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>